<commit_message>
First implementation of regexp parser methods. Untested, doesnt do anything currently. No compiler yet. Should handle precedence as per instructions. Updated grammar sheet, more detail, better precedence.
</commit_message>
<xml_diff>
--- a/ass4 grammar.xlsx
+++ b/ass4 grammar.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="51">
   <si>
     <t>F -&gt; α</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Factor can be a literal</t>
   </si>
   <si>
-    <t>down</t>
+    <t>matching</t>
   </si>
   <si>
     <t>Factor: granular, base level, atomic unit, literals, brackets, evaluated first on it own</t>
@@ -82,16 +82,19 @@
     <t>alternation</t>
   </si>
   <si>
-    <t>T -&gt; \S</t>
-  </si>
-  <si>
-    <t>Term can be an escaped Symbol</t>
+    <t>F -&gt; \S</t>
+  </si>
+  <si>
+    <t>Factor can be an escaped Symbol</t>
+  </si>
+  <si>
+    <t>escape</t>
   </si>
   <si>
     <t>S -&gt; s</t>
   </si>
   <si>
-    <t>Symbol matches any typeable symbol</t>
+    <t>Symbol can be any typeable symbol</t>
   </si>
   <si>
     <t>T -&gt; [D]</t>
@@ -100,9 +103,6 @@
     <t>A term can be a disjunctive list of literals</t>
   </si>
   <si>
-    <t>literal list</t>
-  </si>
-  <si>
     <t>D -&gt; α</t>
   </si>
   <si>
@@ -128,13 +128,49 @@
   </si>
   <si>
     <t>concat</t>
+  </si>
+  <si>
+    <t>first precendence pass</t>
+  </si>
+  <si>
+    <t>Final precedence pass</t>
+  </si>
+  <si>
+    <t>Grammar</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>precedence</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>Factor can be an escaped symbol</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -142,6 +178,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -156,8 +204,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB4A7D6"/>
-        <bgColor rgb="FFB4A7D6"/>
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -180,8 +228,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
+        <fgColor rgb="FFA64D79"/>
+        <bgColor rgb="FFA64D79"/>
       </patternFill>
     </fill>
     <fill>
@@ -197,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -221,6 +269,29 @@
     </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,16 +616,16 @@
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
+      <c r="C9" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
@@ -562,13 +633,13 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -578,8 +649,8 @@
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
+      <c r="C12" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13">
@@ -589,8 +660,8 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>29</v>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14">
@@ -613,6 +684,369 @@
       </c>
       <c r="C15" s="7" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="13"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="13"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>